<commit_message>
Adicionando a estrutura fundamental do HTML e CSS, adicionando melhorias e testes no processo de ETL
</commit_message>
<xml_diff>
--- a/dados_producao/Tabela_fato_em_producao.xlsx
+++ b/dados_producao/Tabela_fato_em_producao.xlsx
@@ -39,7 +39,7 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>ID_transacao</t>
+    <t>ID_Transacao</t>
   </si>
 </sst>
 </file>
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -516,6 +516,52 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>45964</v>
       </c>
     </row>

</xml_diff>